<commit_message>
Rediseno completo UI MovPer: login, registro, checklist, config - profesional con Inter font, SVG icons, rename MobPer->MovPer, fix endpoint references
</commit_message>
<xml_diff>
--- a/webapp/output/mobper/MobPer_8490_20260116.xlsx
+++ b/webapp/output/mobper/MobPer_8490_20260116.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Downloads\debug biostar para checadores\webapp\output\mobper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0564D15A-2881-4466-A45D-D2F8413EDA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BADD794-CD40-4090-AC62-306AEB56572F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,7 +335,7 @@
     <t>RAÚL CETINA</t>
   </si>
   <si>
-    <t>DISEÑO</t>
+    <t>IT</t>
   </si>
   <si>
     <t>16,19,20,21,22,27,28 de enero</t>

</xml_diff>